<commit_message>
Hardware design for door state detection
</commit_message>
<xml_diff>
--- a/Documents/GANTT.xlsx
+++ b/Documents/GANTT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\studenthome.cis.strath.ac.uk\homes\system\Windows\My Documents\Pi Stuff\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\studenthome.cis.strath.ac.uk\homes\system\Windows\My Documents\cs413\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,9 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="41">
   <si>
-    <t>C.O.O.L.S.</t>
-  </si>
-  <si>
     <t>ACTIVITY</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>Create user Interface design</t>
+  </si>
+  <si>
+    <t>F.R.I.D.G.E.S</t>
   </si>
 </sst>
 </file>
@@ -688,10 +688,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A3:BJ42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,7 +705,7 @@
   <sheetData>
     <row r="3" spans="1:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -729,17 +732,17 @@
     <row r="6" spans="1:62" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
       <c r="G7" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -748,7 +751,7 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
@@ -757,7 +760,7 @@
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
       <c r="U7" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V7" s="5"/>
       <c r="W7" s="6"/>
@@ -766,7 +769,7 @@
       <c r="Z7" s="6"/>
       <c r="AA7" s="6"/>
       <c r="AB7" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AC7" s="6"/>
       <c r="AD7" s="6"/>
@@ -775,7 +778,7 @@
       <c r="AG7" s="6"/>
       <c r="AH7" s="6"/>
       <c r="AI7" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AJ7" s="6"/>
       <c r="AK7" s="6"/>
@@ -784,7 +787,7 @@
       <c r="AN7" s="6"/>
       <c r="AO7" s="6"/>
       <c r="AP7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AQ7" s="6"/>
       <c r="AR7" s="6"/>
@@ -793,7 +796,7 @@
       <c r="AU7" s="6"/>
       <c r="AV7" s="6"/>
       <c r="AW7" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AX7" s="6"/>
       <c r="AY7" s="6"/>
@@ -802,7 +805,7 @@
       <c r="BB7" s="6"/>
       <c r="BC7" s="6"/>
       <c r="BD7" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BE7" s="6"/>
       <c r="BF7" s="6"/>
@@ -815,189 +818,189 @@
       <c r="A8" s="8"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>12</v>
-      </c>
       <c r="E8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="H8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="O8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="P8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="Q8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="R8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="13" t="s">
+      <c r="S8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="U8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="V8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="W8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="X8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="L8" s="13" t="s">
+      <c r="Z8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="AC8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="8" t="s">
+      <c r="AJ8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="8" t="s">
+      <c r="AL8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q8" s="8" t="s">
+      <c r="AN8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AR8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="R8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="S8" s="8" t="s">
+      <c r="AU8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="T8" s="8" t="s">
+      <c r="AX8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AY8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AZ8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="BA8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="BC8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="BD8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="U8" s="8" t="s">
+      <c r="BE8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="BF8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="V8" s="8" t="s">
+      <c r="BG8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="BH8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="W8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="X8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AI8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AO8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AP8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="AQ8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AR8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="AS8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AT8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AV8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AW8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="AX8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AY8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="AZ8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="BA8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="BB8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="BC8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="BD8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="BF8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="BG8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="BH8" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="BI8" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BJ8" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -1014,15 +1017,15 @@
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -1032,22 +1035,22 @@
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -1064,7 +1067,7 @@
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W16" s="9"/>
       <c r="X16" s="9"/>
@@ -1074,7 +1077,7 @@
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
@@ -1084,22 +1087,22 @@
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
         <v>23</v>
-      </c>
-      <c r="B19" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
@@ -1111,7 +1114,7 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
@@ -1119,15 +1122,15 @@
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -1136,7 +1139,7 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
@@ -1148,7 +1151,7 @@
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R27" s="9"/>
       <c r="U27" s="9"/>
@@ -1156,22 +1159,22 @@
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
         <v>34</v>
-      </c>
-      <c r="B29" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -1181,7 +1184,7 @@
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N32" s="9"/>
       <c r="O32" s="9"/>
@@ -1189,17 +1192,17 @@
     </row>
     <row r="34" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AB37" s="9"/>
       <c r="AC37" s="9"/>
@@ -1207,7 +1210,7 @@
     </row>
     <row r="38" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AE38" s="9"/>
       <c r="AF38" s="9"/>
@@ -1222,7 +1225,7 @@
     </row>
     <row r="39" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AP39" s="9"/>
       <c r="AQ39" s="9"/>
@@ -1232,7 +1235,7 @@
     </row>
     <row r="42" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AW42" s="9"/>
       <c r="AX42" s="9"/>
@@ -1254,6 +1257,7 @@
       <formula>C$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="21" scale="56" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>